<commit_message>
menambahkan export xlsx pada stock Out
</commit_message>
<xml_diff>
--- a/DataStok.xlsx
+++ b/DataStok.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Tanggal Keluar</t>
+  </si>
   <si>
     <t>Lokasi</t>
   </si>
@@ -22,16 +28,16 @@
     <t>Kode</t>
   </si>
   <si>
-    <t>Nama</t>
+    <t>Nama Barang</t>
   </si>
   <si>
     <t>Unit</t>
   </si>
   <si>
-    <t>Keluar</t>
-  </si>
-  <si>
-    <t>Total</t>
+    <t>Barang Keluar</t>
+  </si>
+  <si>
+    <t>Total Barang</t>
   </si>
   <si>
     <t>ID</t>
@@ -40,7 +46,7 @@
     <t>Tangerang</t>
   </si>
   <si>
-    <t/>
+    <t>12345</t>
   </si>
   <si>
     <t>sukasuka</t>
@@ -81,8 +87,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="false">
+      <alignment/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,13 +387,19 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45242.950240115744</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -392,22 +407,28 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>350000</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45242.95028357639</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -415,22 +436,28 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>350000</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45242.950316724535</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -438,22 +465,28 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>350000</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>2</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45242.95065928241</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -461,22 +494,28 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
         <v>10000</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>340000</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45242.950700381945</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -484,22 +523,28 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6">
         <v>10000</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>330000</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>2</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45243.25965025463</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -507,13 +552,48 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7">
         <v>10000</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>320000</v>
       </c>
-      <c r="G7">
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45243.848213032405</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>10000</v>
+      </c>
+      <c r="H8">
+        <v>310000</v>
+      </c>
+      <c r="I8">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
memperbaiki panjang kolom  pada  export xlsx pada stock Out
</commit_message>
<xml_diff>
--- a/DataStok.xlsx
+++ b/DataStok.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>No</t>
   </si>
@@ -43,6 +43,9 @@
     <t>ID</t>
   </si>
   <si>
+    <t>Student Examp Score</t>
+  </si>
+  <si>
     <t>Tangerang</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t>dus</t>
+  </si>
+  <si>
+    <t>Kabel RJ45</t>
   </si>
 </sst>
 </file>
@@ -364,6 +370,16 @@
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="true" max="1" min="1" width="21"/>
+    <col customWidth="true" max="3" min="2" width="16"/>
+    <col customWidth="true" max="4" min="4" width="11"/>
+    <col customWidth="true" max="5" min="5" width="13"/>
+    <col customWidth="true" max="6" min="6" width="12"/>
+    <col customWidth="true" max="7" min="7" width="15"/>
+    <col customWidth="true" max="8" min="8" width="14"/>
+    <col customWidth="true" max="9" min="9" width="8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -395,14 +411,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>45242.950240115744</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
+      <c r="C2" s="1">
+        <v>45242.9502401157</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -413,25 +429,28 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>350000</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45242.95028357639</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45242.9502835764</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -442,25 +461,28 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>350000</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>45242.950316724535</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
+      <c r="C4" s="1">
+        <v>45242.9503167245</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -471,25 +493,28 @@
       <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>350000</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>45242.95065928241</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
+      <c r="C5" s="1">
+        <v>45242.9506592824</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -500,25 +525,28 @@
       <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
         <v>10000</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>340000</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>45242.950700381945</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
+      <c r="C6" s="1">
+        <v>45242.9507003819</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -529,25 +557,28 @@
       <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6">
         <v>10000</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>330000</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>2</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>45243.25965025463</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
+      <c r="C7" s="1">
+        <v>45243.2596502546</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -558,25 +589,28 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7">
         <v>10000</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>320000</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
-        <v>45243.848213032405</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
+      <c r="C8" s="1">
+        <v>45243.8482130324</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -587,14 +621,49 @@
       <c r="F8" t="s">
         <v>12</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8">
         <v>10000</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>310000</v>
       </c>
-      <c r="I8">
-        <v>2</v>
+      <c r="J8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45243.8699079051</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
memperbaiki panjang header judul pada  export xlsx pada stock Out
</commit_message>
<xml_diff>
--- a/DataStok.xlsx
+++ b/DataStok.xlsx
@@ -16,6 +16,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
+    <t>Data Stok - Rekapitulasi Barang Keluar</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
@@ -41,9 +44,6 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>Student Examp Score</t>
   </si>
   <si>
     <t>Tangerang</t>
@@ -65,10 +65,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="14"/>
+      <color/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -93,8 +100,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="false">
       <alignment/>
     </xf>
@@ -370,302 +380,284 @@
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col customWidth="true" max="1" min="1" width="21"/>
-    <col customWidth="true" max="3" min="2" width="16"/>
-    <col customWidth="true" max="4" min="4" width="11"/>
-    <col customWidth="true" max="5" min="5" width="13"/>
-    <col customWidth="true" max="6" min="6" width="12"/>
-    <col customWidth="true" max="7" min="7" width="15"/>
-    <col customWidth="true" max="8" min="8" width="14"/>
-    <col customWidth="true" max="9" min="9" width="8"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
+    </row>
+    <row r="3">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>45242.9502401157</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B3" s="2">
+        <v>45242.950240115744</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="H3">
         <v>350000</v>
       </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>45242.9502835764</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45242.95028357639</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3">
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="I3">
+      <c r="H4">
         <v>350000</v>
       </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
-        <v>45242.9503167245</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B5" s="2">
+        <v>45242.950316724535</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4">
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="H5">
         <v>350000</v>
       </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
+      <c r="I5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>45242.9506592824</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="B6" s="2">
+        <v>45242.95065928241</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5">
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
         <v>10000</v>
       </c>
-      <c r="I5">
+      <c r="H6">
         <v>340000</v>
       </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
-        <v>45242.9507003819</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="B7" s="2">
+        <v>45242.950700381945</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6">
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
         <v>10000</v>
       </c>
-      <c r="I6">
+      <c r="H7">
         <v>330000</v>
       </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
-        <v>45243.2596502546</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="B8" s="2">
+        <v>45243.25965025463</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
         <v>12</v>
       </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7">
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
         <v>10000</v>
       </c>
-      <c r="I7">
+      <c r="H8">
         <v>320000</v>
       </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
+      <c r="I8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
-        <v>45243.8482130324</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="B9" s="2">
+        <v>45243.848213032405</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
         <v>12</v>
       </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8">
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
         <v>10000</v>
       </c>
-      <c r="I8">
+      <c r="H9">
         <v>310000</v>
       </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="C9" s="1">
-        <v>45243.8699079051</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="B10" s="2">
+        <v>45243.86990790509</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9">
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
         <v>20</v>
       </c>
-      <c r="I9">
+      <c r="H10">
         <v>8</v>
       </c>
-      <c r="J9">
+      <c r="I10">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
 </worksheet>
 </file>
</xml_diff>